<commit_message>
tests for benchmark output
</commit_message>
<xml_diff>
--- a/tests/TestFiles/expoutput/Benchmarks_Configuration/ITER_1D.xlsx
+++ b/tests/TestFiles/expoutput/Benchmarks_Configuration/ITER_1D.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laghi\Documents\03_dottorato\04_F4E\01_JADE\Code\Default Settings\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JADE-linux\Code\tests\TestFiles\expoutput\Benchmarks_Configuration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD426A26-4FB7-416C-A722-5DBBD13BAB73}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9CF0D0E-8373-4EE1-9BD5-8DCD2E7584F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{B2FBD261-A6D7-48D0-8F16-20EC1D949C31}"/>
+    <workbookView xWindow="1635" yWindow="1620" windowWidth="18000" windowHeight="9360" activeTab="1" xr2:uid="{B2FBD261-A6D7-48D0-8F16-20EC1D949C31}"/>
   </bookViews>
   <sheets>
     <sheet name="Excel" sheetId="1" r:id="rId1"/>
@@ -264,7 +264,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -281,16 +281,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -301,7 +295,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -317,7 +311,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -627,22 +621,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1009,7 +1003,7 @@
       <c r="E22" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F22" s="6">
+      <c r="F22" s="1">
         <v>20</v>
       </c>
     </row>
@@ -1075,358 +1069,358 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="D4" sqref="D2:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="8"/>
-    <col min="2" max="2" width="26.7109375" style="8" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" style="8" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" style="8" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" style="8" customWidth="1"/>
-    <col min="6" max="16384" width="8.85546875" style="8"/>
+    <col min="1" max="1" width="8.85546875" style="7"/>
+    <col min="2" max="2" width="26.7109375" style="7" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" style="7" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" style="7" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="9" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="8">
+      <c r="A2" s="7">
         <v>4</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
+        <v>14</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="7">
+        <v>6</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="8">
-        <v>14</v>
-      </c>
-      <c r="B3" s="8" t="s">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
+        <v>16</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
+        <v>26</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
+        <v>24</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
+        <v>34</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
+        <v>44</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
+        <v>54</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
+        <v>64</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
+        <v>74</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
+        <v>84</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="7">
+        <v>94</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="7">
+        <v>104</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="7">
+        <v>114</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="7">
+        <v>124</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="7">
+        <v>134</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="7">
+        <v>144</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="7">
+        <v>154</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="7">
+        <v>164</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="7">
+        <v>174</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="7">
+        <v>204</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="7">
+        <v>214</v>
+      </c>
+      <c r="B24" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C24" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="8">
-        <v>6</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="8">
-        <v>16</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="8">
-        <v>26</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="8">
-        <v>24</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="8">
-        <v>34</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="8">
-        <v>44</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="8">
-        <v>54</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="8">
-        <v>64</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="8">
-        <v>74</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="8">
-        <v>84</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="8">
-        <v>94</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="8">
-        <v>104</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="8">
-        <v>114</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="8">
-        <v>124</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="8">
-        <v>134</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="8">
-        <v>144</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="8">
-        <v>154</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="8">
-        <v>164</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="8">
-        <v>174</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E22" s="8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="8">
-        <v>204</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="8">
-        <v>214</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E24" s="8" t="s">
+      <c r="D24" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E24" s="7" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>